<commit_message>
Updated field dictionary, updated vignette query, release note placeholders
</commit_message>
<xml_diff>
--- a/vignettes/cvtdb_field_dictionary.xlsx
+++ b/vignettes/cvtdb_field_dictionary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdbLoad/vignettes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="11_29E9DED48F79A8D366075C52F37BD2729AC9D7E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C22C6F79-1FBD-4255-8C76-EAAD6AB9FA52}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="11_29E9DED48F79A8D366075C52F37BD2729AC9D7E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B1BCB2A-AECD-444B-83A9-20ED827D1780}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="378">
   <si>
     <t>table_name</t>
   </si>
@@ -1148,13 +1148,22 @@
   </si>
   <si>
     <t>Original value reported in the extraction document. See corresponding chemicals table entry using fk_dosed_chemical_id field</t>
+  </si>
+  <si>
+    <t>Unique identifier assigned to a concept within the domain of mammalian experimentation as designated in the concept_identifier_dictionary</t>
+  </si>
+  <si>
+    <t>Name of an authoritative vocabulary, dictionary, or ontology which defines concepts within the domain of mammalian experimentation</t>
+  </si>
+  <si>
+    <t>Label or name used by the concept_identifier_dictionary to describe the concept_identifier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1168,6 +1177,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1191,7 +1206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1199,6 +1214,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1503,12 +1519,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:E272"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1537,7 +1550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1551,7 +1564,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1562,12 +1575,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1577,16 +1593,22 @@
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1597,7 +1619,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1608,7 +1630,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -1619,7 +1641,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -1633,7 +1655,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -1644,12 +1666,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1659,16 +1684,22 @@
       <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -1679,7 +1710,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -1690,7 +1721,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -1701,7 +1732,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
@@ -1715,7 +1746,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
@@ -1726,12 +1757,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1741,16 +1775,22 @@
       <c r="B21" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
@@ -1761,7 +1801,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
@@ -1772,7 +1812,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
@@ -1783,7 +1823,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
@@ -1794,7 +1834,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
@@ -1805,7 +1845,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>30</v>
       </c>
@@ -1816,7 +1856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>30</v>
       </c>
@@ -1833,7 +1873,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>30</v>
       </c>
@@ -1844,7 +1884,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
@@ -1855,7 +1895,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -1866,7 +1906,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>30</v>
       </c>
@@ -1877,7 +1917,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>30</v>
       </c>
@@ -1888,7 +1928,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>30</v>
       </c>
@@ -1899,7 +1939,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>30</v>
       </c>
@@ -1910,7 +1950,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>46</v>
       </c>
@@ -1924,7 +1964,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>46</v>
       </c>
@@ -1935,12 +1975,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1950,16 +1993,22 @@
       <c r="B40" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C40" s="3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>46</v>
       </c>
@@ -1970,7 +2019,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>46</v>
       </c>
@@ -1984,7 +2033,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>46</v>
       </c>
@@ -1995,7 +2044,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>46</v>
       </c>
@@ -2006,7 +2055,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>46</v>
       </c>
@@ -2023,7 +2072,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>55</v>
       </c>
@@ -2037,7 +2086,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>55</v>
       </c>
@@ -2051,7 +2100,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>55</v>
       </c>
@@ -2062,7 +2111,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>55</v>
       </c>
@@ -2073,7 +2122,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>55</v>
       </c>
@@ -2084,7 +2133,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>55</v>
       </c>
@@ -2095,7 +2144,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>55</v>
       </c>
@@ -2106,7 +2155,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>55</v>
       </c>
@@ -2117,7 +2166,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>55</v>
       </c>
@@ -2128,7 +2177,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>55</v>
       </c>
@@ -2139,7 +2188,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>55</v>
       </c>
@@ -2150,7 +2199,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>55</v>
       </c>
@@ -2161,7 +2210,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>55</v>
       </c>
@@ -2172,7 +2221,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>55</v>
       </c>
@@ -2189,7 +2238,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>55</v>
       </c>
@@ -2200,7 +2249,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>55</v>
       </c>
@@ -2211,7 +2260,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>55</v>
       </c>
@@ -2222,7 +2271,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>55</v>
       </c>
@@ -2233,7 +2282,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>55</v>
       </c>
@@ -2244,7 +2293,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>55</v>
       </c>
@@ -2255,7 +2304,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>55</v>
       </c>
@@ -2266,7 +2315,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>91</v>
       </c>
@@ -2277,7 +2326,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>91</v>
       </c>
@@ -2288,7 +2337,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>91</v>
       </c>
@@ -2299,7 +2348,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>91</v>
       </c>
@@ -2310,7 +2359,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>91</v>
       </c>
@@ -2321,7 +2370,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>91</v>
       </c>
@@ -2332,7 +2381,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>91</v>
       </c>
@@ -2343,7 +2392,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>91</v>
       </c>
@@ -2354,7 +2403,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>91</v>
       </c>
@@ -2365,7 +2414,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>91</v>
       </c>
@@ -2376,7 +2425,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>91</v>
       </c>
@@ -2387,7 +2436,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>100</v>
       </c>
@@ -2398,7 +2447,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>100</v>
       </c>
@@ -2409,7 +2458,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>100</v>
       </c>
@@ -2420,7 +2469,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>100</v>
       </c>
@@ -2431,7 +2480,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>100</v>
       </c>
@@ -2442,7 +2491,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>100</v>
       </c>
@@ -2453,7 +2502,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>100</v>
       </c>
@@ -2467,7 +2516,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>100</v>
       </c>
@@ -2481,7 +2530,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>100</v>
       </c>
@@ -2498,7 +2547,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>100</v>
       </c>
@@ -2509,7 +2558,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>100</v>
       </c>
@@ -2523,7 +2572,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>100</v>
       </c>
@@ -2534,7 +2583,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>100</v>
       </c>
@@ -2545,7 +2594,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>100</v>
       </c>
@@ -2562,7 +2611,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>100</v>
       </c>
@@ -2576,7 +2625,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>100</v>
       </c>
@@ -2587,7 +2636,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>100</v>
       </c>
@@ -2598,7 +2647,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>100</v>
       </c>
@@ -2609,7 +2658,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>100</v>
       </c>
@@ -2620,7 +2669,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>100</v>
       </c>
@@ -2631,7 +2680,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>100</v>
       </c>
@@ -2642,7 +2691,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>100</v>
       </c>
@@ -2653,7 +2702,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>100</v>
       </c>
@@ -2664,7 +2713,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>100</v>
       </c>
@@ -2681,7 +2730,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>100</v>
       </c>
@@ -2692,7 +2741,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>100</v>
       </c>
@@ -2706,7 +2755,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>100</v>
       </c>
@@ -2723,7 +2772,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>100</v>
       </c>
@@ -2740,7 +2789,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>100</v>
       </c>
@@ -2751,7 +2800,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>100</v>
       </c>
@@ -2762,7 +2811,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>100</v>
       </c>
@@ -2773,7 +2822,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>152</v>
       </c>
@@ -2784,7 +2833,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>152</v>
       </c>
@@ -2795,7 +2844,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>152</v>
       </c>
@@ -2806,7 +2855,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>152</v>
       </c>
@@ -2817,7 +2866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>152</v>
       </c>
@@ -2828,7 +2877,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>152</v>
       </c>
@@ -2842,12 +2891,15 @@
         <v>159</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>160</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -2857,16 +2909,22 @@
       <c r="B117" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C117" s="3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>160</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C118" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>160</v>
       </c>
@@ -2877,7 +2935,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>160</v>
       </c>
@@ -2891,7 +2949,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>160</v>
       </c>
@@ -2902,7 +2960,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>160</v>
       </c>
@@ -2913,7 +2971,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>160</v>
       </c>
@@ -2924,7 +2982,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>165</v>
       </c>
@@ -2935,7 +2993,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>165</v>
       </c>
@@ -2946,7 +3004,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>165</v>
       </c>
@@ -2957,7 +3015,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>165</v>
       </c>
@@ -2968,7 +3026,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>165</v>
       </c>
@@ -2979,7 +3037,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>165</v>
       </c>
@@ -2993,7 +3051,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>165</v>
       </c>
@@ -3004,7 +3062,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>165</v>
       </c>
@@ -3015,7 +3073,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>165</v>
       </c>
@@ -3026,7 +3084,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>165</v>
       </c>
@@ -3037,7 +3095,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>165</v>
       </c>
@@ -3048,7 +3106,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>165</v>
       </c>
@@ -3062,7 +3120,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>165</v>
       </c>
@@ -3076,7 +3134,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>165</v>
       </c>
@@ -3090,7 +3148,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>165</v>
       </c>
@@ -3101,7 +3159,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>165</v>
       </c>
@@ -3112,7 +3170,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>165</v>
       </c>
@@ -3123,7 +3181,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>165</v>
       </c>
@@ -3134,7 +3192,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>165</v>
       </c>
@@ -3145,7 +3203,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>165</v>
       </c>
@@ -3156,7 +3214,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>165</v>
       </c>
@@ -3167,7 +3225,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>165</v>
       </c>
@@ -3181,7 +3239,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>165</v>
       </c>
@@ -3198,7 +3256,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>165</v>
       </c>
@@ -3209,7 +3267,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>165</v>
       </c>
@@ -3220,7 +3278,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>165</v>
       </c>
@@ -3234,7 +3292,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>165</v>
       </c>
@@ -3245,7 +3303,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>165</v>
       </c>
@@ -3256,7 +3314,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>165</v>
       </c>
@@ -3267,7 +3325,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>165</v>
       </c>
@@ -3278,7 +3336,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>165</v>
       </c>
@@ -3289,7 +3347,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>165</v>
       </c>
@@ -3300,7 +3358,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>165</v>
       </c>
@@ -3311,7 +3369,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>165</v>
       </c>
@@ -3325,7 +3383,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="158" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>165</v>
       </c>
@@ -3339,7 +3397,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="159" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>165</v>
       </c>
@@ -3353,7 +3411,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>165</v>
       </c>
@@ -3367,7 +3425,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>221</v>
       </c>
@@ -3378,7 +3436,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>221</v>
       </c>
@@ -3389,7 +3447,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="163" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>221</v>
       </c>
@@ -3400,7 +3458,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="164" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>221</v>
       </c>
@@ -3411,7 +3469,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>221</v>
       </c>
@@ -3422,7 +3480,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>221</v>
       </c>
@@ -3433,7 +3491,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>221</v>
       </c>
@@ -3444,7 +3502,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>221</v>
       </c>
@@ -3455,7 +3513,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>221</v>
       </c>
@@ -3466,7 +3524,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>221</v>
       </c>
@@ -3477,7 +3535,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="171" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>221</v>
       </c>
@@ -3488,7 +3546,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="172" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>221</v>
       </c>
@@ -3499,7 +3557,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="173" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>221</v>
       </c>
@@ -3510,7 +3568,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>221</v>
       </c>
@@ -3524,7 +3582,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="175" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>221</v>
       </c>
@@ -3538,7 +3596,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>221</v>
       </c>
@@ -3549,7 +3607,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="177" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>221</v>
       </c>
@@ -3560,7 +3618,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="178" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>221</v>
       </c>
@@ -3571,7 +3629,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="179" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>221</v>
       </c>
@@ -3582,7 +3640,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="180" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>221</v>
       </c>
@@ -3593,7 +3651,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="181" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>221</v>
       </c>
@@ -3604,7 +3662,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="182" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>221</v>
       </c>
@@ -3615,7 +3673,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>221</v>
       </c>
@@ -3626,7 +3684,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="184" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>221</v>
       </c>
@@ -3637,7 +3695,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>221</v>
       </c>
@@ -3648,7 +3706,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>221</v>
       </c>
@@ -3659,7 +3717,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="187" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>221</v>
       </c>
@@ -3670,7 +3728,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>221</v>
       </c>
@@ -3681,7 +3739,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="189" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>221</v>
       </c>
@@ -3695,7 +3753,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>221</v>
       </c>
@@ -3706,7 +3764,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="191" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>221</v>
       </c>
@@ -3717,7 +3775,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="192" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>221</v>
       </c>
@@ -3731,7 +3789,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="193" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>221</v>
       </c>
@@ -3745,7 +3803,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="194" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>221</v>
       </c>
@@ -3756,7 +3814,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="195" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>221</v>
       </c>
@@ -3767,7 +3825,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="196" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>221</v>
       </c>
@@ -3778,7 +3836,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="197" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>221</v>
       </c>
@@ -3789,7 +3847,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="198" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>221</v>
       </c>
@@ -3800,7 +3858,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="199" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>221</v>
       </c>
@@ -3811,7 +3869,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="200" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>221</v>
       </c>
@@ -3822,7 +3880,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="201" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>221</v>
       </c>
@@ -3833,7 +3891,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="202" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>221</v>
       </c>
@@ -3844,7 +3902,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="203" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>221</v>
       </c>
@@ -3855,7 +3913,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="204" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>221</v>
       </c>
@@ -3866,7 +3924,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="205" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>221</v>
       </c>
@@ -3877,7 +3935,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="206" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>221</v>
       </c>
@@ -3888,7 +3946,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="207" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>221</v>
       </c>
@@ -3899,7 +3957,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="208" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>221</v>
       </c>
@@ -3910,7 +3968,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="209" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>221</v>
       </c>
@@ -3924,7 +3982,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="210" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>221</v>
       </c>
@@ -3935,7 +3993,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="211" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>221</v>
       </c>
@@ -3946,7 +4004,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="212" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>221</v>
       </c>
@@ -3957,7 +4015,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>221</v>
       </c>
@@ -3968,7 +4026,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>221</v>
       </c>
@@ -3979,7 +4037,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="215" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>221</v>
       </c>
@@ -3990,7 +4048,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="216" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>303</v>
       </c>
@@ -4001,7 +4059,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="217" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>303</v>
       </c>
@@ -4015,7 +4073,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="218" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>303</v>
       </c>
@@ -4026,7 +4084,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="219" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>303</v>
       </c>
@@ -4037,7 +4095,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="220" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>303</v>
       </c>
@@ -4048,7 +4106,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="221" spans="1:4" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>303</v>
       </c>
@@ -4059,7 +4117,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="222" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>303</v>
       </c>
@@ -4070,7 +4128,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="223" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>303</v>
       </c>
@@ -4081,7 +4139,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="224" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>303</v>
       </c>
@@ -4092,7 +4150,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="225" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>303</v>
       </c>
@@ -4103,7 +4161,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="226" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>303</v>
       </c>
@@ -4114,7 +4172,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="227" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>303</v>
       </c>
@@ -4125,7 +4183,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="228" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>303</v>
       </c>
@@ -4136,7 +4194,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="229" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>303</v>
       </c>
@@ -4147,7 +4205,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="230" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>303</v>
       </c>
@@ -4158,7 +4216,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="231" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>303</v>
       </c>
@@ -4169,7 +4227,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="232" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>303</v>
       </c>
@@ -4180,7 +4238,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="233" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>303</v>
       </c>
@@ -4191,7 +4249,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="234" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>303</v>
       </c>
@@ -4202,7 +4260,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="235" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>303</v>
       </c>
@@ -4213,7 +4271,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="236" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>303</v>
       </c>
@@ -4227,7 +4285,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="237" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>303</v>
       </c>
@@ -4238,7 +4296,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="238" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>303</v>
       </c>
@@ -4249,7 +4307,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="239" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>334</v>
       </c>
@@ -4263,7 +4321,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="240" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>334</v>
       </c>
@@ -4274,7 +4332,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="241" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>334</v>
       </c>
@@ -4285,7 +4343,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="242" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>334</v>
       </c>
@@ -4296,7 +4354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="243" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>334</v>
       </c>
@@ -4307,7 +4365,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="244" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>334</v>
       </c>
@@ -4318,7 +4376,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="245" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
         <v>334</v>
       </c>
@@ -4329,7 +4387,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="246" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>334</v>
       </c>
@@ -4340,7 +4398,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="247" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>334</v>
       </c>
@@ -4351,7 +4409,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="248" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>334</v>
       </c>
@@ -4365,7 +4423,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="249" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>334</v>
       </c>
@@ -4376,7 +4434,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="250" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>334</v>
       </c>
@@ -4387,7 +4445,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="251" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>334</v>
       </c>
@@ -4398,7 +4456,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="252" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>334</v>
       </c>
@@ -4409,7 +4467,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="253" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>334</v>
       </c>
@@ -4420,7 +4478,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="254" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>334</v>
       </c>
@@ -4431,7 +4489,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="255" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>334</v>
       </c>
@@ -4442,7 +4500,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="256" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>334</v>
       </c>
@@ -4453,7 +4511,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="257" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>334</v>
       </c>
@@ -4464,7 +4522,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="258" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>334</v>
       </c>
@@ -4475,7 +4533,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="259" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>334</v>
       </c>
@@ -4486,7 +4544,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="260" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>334</v>
       </c>
@@ -4497,7 +4555,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="261" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>362</v>
       </c>
@@ -4508,7 +4566,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="262" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>362</v>
       </c>
@@ -4519,7 +4577,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="263" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>362</v>
       </c>
@@ -4530,7 +4588,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="264" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>362</v>
       </c>
@@ -4541,7 +4599,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="265" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>362</v>
       </c>
@@ -4552,7 +4610,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="266" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>362</v>
       </c>
@@ -4563,7 +4621,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="267" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>365</v>
       </c>
@@ -4574,7 +4632,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="268" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>365</v>
       </c>
@@ -4585,7 +4643,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="269" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>365</v>
       </c>
@@ -4596,7 +4654,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="270" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>365</v>
       </c>
@@ -4607,7 +4665,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="271" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
         <v>365</v>
       </c>
@@ -4618,7 +4676,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="272" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>365</v>
       </c>
@@ -4630,11 +4688,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E272" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="2">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E272" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Additional summaries, visualizations, and updated release notes
</commit_message>
<xml_diff>
--- a/vignettes/cvtdb_field_dictionary.xlsx
+++ b/vignettes/cvtdb_field_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdbLoad/vignettes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="11_29E9DED48F79A8D366075C52F37BD2729AC9D7E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B1BCB2A-AECD-444B-83A9-20ED827D1780}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="11_29E9DED48F79A8D366075C52F37BD2729AC9D7E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56908DF2-E445-43C4-8C08-9F289DBAEB7C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34005" yWindow="1275" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="379">
   <si>
     <t>table_name</t>
   </si>
@@ -1157,6 +1157,9 @@
   </si>
   <si>
     <t>Label or name used by the concept_identifier_dictionary to describe the concept_identifier</t>
+  </si>
+  <si>
+    <t>Deprecated, field is no longer in use and weight_kg is not affected by this flag</t>
   </si>
 </sst>
 </file>
@@ -1519,9 +1522,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E272"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E236" sqref="E236"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1550,7 +1556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1564,7 +1570,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1575,7 +1581,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1586,7 +1592,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1597,7 +1603,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1608,7 +1614,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1619,7 +1625,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1630,7 +1636,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -1641,7 +1647,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -1655,7 +1661,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -1666,7 +1672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -1677,7 +1683,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -1688,7 +1694,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -1699,7 +1705,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -1710,7 +1716,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -1721,7 +1727,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -1732,7 +1738,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
@@ -1746,7 +1752,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
@@ -1757,7 +1763,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
@@ -1768,7 +1774,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -1779,7 +1785,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
@@ -1790,7 +1796,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
@@ -1801,7 +1807,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
@@ -1812,7 +1818,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
@@ -1823,7 +1829,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
@@ -1834,7 +1840,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
@@ -1845,7 +1851,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>30</v>
       </c>
@@ -1856,7 +1862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>30</v>
       </c>
@@ -1873,7 +1879,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>30</v>
       </c>
@@ -1884,7 +1890,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
@@ -1895,7 +1901,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -1906,7 +1912,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>30</v>
       </c>
@@ -1917,7 +1923,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>30</v>
       </c>
@@ -1928,7 +1934,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>30</v>
       </c>
@@ -1939,7 +1945,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>30</v>
       </c>
@@ -1950,7 +1956,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>46</v>
       </c>
@@ -1964,7 +1970,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>46</v>
       </c>
@@ -1975,7 +1981,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>46</v>
       </c>
@@ -1986,7 +1992,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>46</v>
       </c>
@@ -1997,7 +2003,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>46</v>
       </c>
@@ -2008,7 +2014,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>46</v>
       </c>
@@ -2019,7 +2025,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>46</v>
       </c>
@@ -2033,7 +2039,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>46</v>
       </c>
@@ -2044,7 +2050,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>46</v>
       </c>
@@ -2055,7 +2061,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>46</v>
       </c>
@@ -2072,7 +2078,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>55</v>
       </c>
@@ -2086,7 +2092,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>55</v>
       </c>
@@ -2100,7 +2106,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>55</v>
       </c>
@@ -2111,7 +2117,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>55</v>
       </c>
@@ -2122,7 +2128,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>55</v>
       </c>
@@ -2133,7 +2139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>55</v>
       </c>
@@ -2144,7 +2150,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>55</v>
       </c>
@@ -2155,7 +2161,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>55</v>
       </c>
@@ -2166,7 +2172,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>55</v>
       </c>
@@ -2177,7 +2183,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>55</v>
       </c>
@@ -2188,7 +2194,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>55</v>
       </c>
@@ -2199,7 +2205,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>55</v>
       </c>
@@ -2210,7 +2216,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>55</v>
       </c>
@@ -2221,7 +2227,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>55</v>
       </c>
@@ -2238,7 +2244,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>55</v>
       </c>
@@ -2249,7 +2255,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>55</v>
       </c>
@@ -2260,7 +2266,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>55</v>
       </c>
@@ -2271,7 +2277,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>55</v>
       </c>
@@ -2282,7 +2288,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>55</v>
       </c>
@@ -2293,7 +2299,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>55</v>
       </c>
@@ -2304,7 +2310,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>55</v>
       </c>
@@ -2315,7 +2321,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>91</v>
       </c>
@@ -2326,7 +2332,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>91</v>
       </c>
@@ -2337,7 +2343,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>91</v>
       </c>
@@ -2348,7 +2354,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>91</v>
       </c>
@@ -2359,7 +2365,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>91</v>
       </c>
@@ -2370,7 +2376,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>91</v>
       </c>
@@ -2381,7 +2387,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>91</v>
       </c>
@@ -2392,7 +2398,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>91</v>
       </c>
@@ -2403,7 +2409,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>91</v>
       </c>
@@ -2414,7 +2420,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>91</v>
       </c>
@@ -2425,7 +2431,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>91</v>
       </c>
@@ -2436,7 +2442,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>100</v>
       </c>
@@ -2447,7 +2453,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>100</v>
       </c>
@@ -2458,7 +2464,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>100</v>
       </c>
@@ -2469,7 +2475,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>100</v>
       </c>
@@ -2480,7 +2486,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>100</v>
       </c>
@@ -2491,7 +2497,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>100</v>
       </c>
@@ -2502,7 +2508,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>100</v>
       </c>
@@ -2516,7 +2522,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>100</v>
       </c>
@@ -2530,7 +2536,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>100</v>
       </c>
@@ -2547,7 +2553,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>100</v>
       </c>
@@ -2558,7 +2564,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>100</v>
       </c>
@@ -2572,7 +2578,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>100</v>
       </c>
@@ -2583,7 +2589,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>100</v>
       </c>
@@ -2594,7 +2600,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>100</v>
       </c>
@@ -2611,7 +2617,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>100</v>
       </c>
@@ -2625,7 +2631,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>100</v>
       </c>
@@ -2636,7 +2642,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>100</v>
       </c>
@@ -2647,7 +2653,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>100</v>
       </c>
@@ -2658,7 +2664,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>100</v>
       </c>
@@ -2669,7 +2675,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>100</v>
       </c>
@@ -2680,7 +2686,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>100</v>
       </c>
@@ -2691,7 +2697,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>100</v>
       </c>
@@ -2702,7 +2708,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>100</v>
       </c>
@@ -2713,7 +2719,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>100</v>
       </c>
@@ -2730,7 +2736,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>100</v>
       </c>
@@ -2741,7 +2747,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>100</v>
       </c>
@@ -2755,7 +2761,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>100</v>
       </c>
@@ -2772,7 +2778,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>100</v>
       </c>
@@ -2789,7 +2795,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>100</v>
       </c>
@@ -2800,7 +2806,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>100</v>
       </c>
@@ -2811,7 +2817,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>100</v>
       </c>
@@ -2822,7 +2828,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>152</v>
       </c>
@@ -2833,7 +2839,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>152</v>
       </c>
@@ -2844,7 +2850,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>152</v>
       </c>
@@ -2855,7 +2861,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>152</v>
       </c>
@@ -2866,7 +2872,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>152</v>
       </c>
@@ -2877,7 +2883,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>152</v>
       </c>
@@ -2891,7 +2897,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>160</v>
       </c>
@@ -2902,7 +2908,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>160</v>
       </c>
@@ -2913,7 +2919,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>160</v>
       </c>
@@ -2924,7 +2930,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>160</v>
       </c>
@@ -2935,7 +2941,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>160</v>
       </c>
@@ -2949,7 +2955,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>160</v>
       </c>
@@ -2960,7 +2966,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>160</v>
       </c>
@@ -2971,7 +2977,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>160</v>
       </c>
@@ -2982,7 +2988,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>165</v>
       </c>
@@ -2993,7 +2999,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>165</v>
       </c>
@@ -3004,7 +3010,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>165</v>
       </c>
@@ -3015,7 +3021,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>165</v>
       </c>
@@ -3026,7 +3032,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>165</v>
       </c>
@@ -3037,7 +3043,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>165</v>
       </c>
@@ -3051,7 +3057,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>165</v>
       </c>
@@ -3062,7 +3068,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>165</v>
       </c>
@@ -3073,7 +3079,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>165</v>
       </c>
@@ -3084,7 +3090,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>165</v>
       </c>
@@ -3095,7 +3101,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>165</v>
       </c>
@@ -3106,7 +3112,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>165</v>
       </c>
@@ -3120,7 +3126,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>165</v>
       </c>
@@ -3134,7 +3140,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>165</v>
       </c>
@@ -3148,7 +3154,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>165</v>
       </c>
@@ -3159,7 +3165,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>165</v>
       </c>
@@ -3170,7 +3176,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>165</v>
       </c>
@@ -3181,7 +3187,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>165</v>
       </c>
@@ -3192,7 +3198,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>165</v>
       </c>
@@ -3203,7 +3209,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>165</v>
       </c>
@@ -3214,7 +3220,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>165</v>
       </c>
@@ -3225,7 +3231,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>165</v>
       </c>
@@ -3239,7 +3245,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>165</v>
       </c>
@@ -3256,7 +3262,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>165</v>
       </c>
@@ -3267,7 +3273,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>165</v>
       </c>
@@ -3278,7 +3284,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>165</v>
       </c>
@@ -3292,7 +3298,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>165</v>
       </c>
@@ -3303,7 +3309,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>165</v>
       </c>
@@ -3314,7 +3320,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>165</v>
       </c>
@@ -3325,7 +3331,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>165</v>
       </c>
@@ -3336,7 +3342,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>165</v>
       </c>
@@ -3347,7 +3353,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>165</v>
       </c>
@@ -3358,7 +3364,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>165</v>
       </c>
@@ -3369,7 +3375,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>165</v>
       </c>
@@ -3383,7 +3389,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>165</v>
       </c>
@@ -3397,7 +3403,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>165</v>
       </c>
@@ -3411,7 +3417,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>165</v>
       </c>
@@ -3425,7 +3431,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>221</v>
       </c>
@@ -3436,7 +3442,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>221</v>
       </c>
@@ -3447,7 +3453,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="163" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>221</v>
       </c>
@@ -3458,7 +3464,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="164" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>221</v>
       </c>
@@ -3469,7 +3475,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>221</v>
       </c>
@@ -3480,7 +3486,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>221</v>
       </c>
@@ -3491,7 +3497,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>221</v>
       </c>
@@ -3502,7 +3508,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>221</v>
       </c>
@@ -3513,7 +3519,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>221</v>
       </c>
@@ -3524,7 +3530,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>221</v>
       </c>
@@ -3535,7 +3541,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>221</v>
       </c>
@@ -3546,7 +3552,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="172" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>221</v>
       </c>
@@ -3557,7 +3563,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>221</v>
       </c>
@@ -3568,7 +3574,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>221</v>
       </c>
@@ -3582,7 +3588,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="175" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>221</v>
       </c>
@@ -3596,7 +3602,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>221</v>
       </c>
@@ -3607,7 +3613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>221</v>
       </c>
@@ -3618,7 +3624,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>221</v>
       </c>
@@ -3629,7 +3635,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>221</v>
       </c>
@@ -3640,7 +3646,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>221</v>
       </c>
@@ -3651,7 +3657,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>221</v>
       </c>
@@ -3662,7 +3668,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>221</v>
       </c>
@@ -3673,7 +3679,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>221</v>
       </c>
@@ -3684,7 +3690,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>221</v>
       </c>
@@ -3695,7 +3701,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>221</v>
       </c>
@@ -3706,7 +3712,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>221</v>
       </c>
@@ -3717,7 +3723,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>221</v>
       </c>
@@ -3728,7 +3734,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>221</v>
       </c>
@@ -3739,7 +3745,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>221</v>
       </c>
@@ -3753,7 +3759,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>221</v>
       </c>
@@ -3764,7 +3770,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>221</v>
       </c>
@@ -3775,7 +3781,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>221</v>
       </c>
@@ -3789,7 +3795,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="193" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>221</v>
       </c>
@@ -3803,7 +3809,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>221</v>
       </c>
@@ -3814,7 +3820,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>221</v>
       </c>
@@ -3825,7 +3831,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>221</v>
       </c>
@@ -3836,7 +3842,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>221</v>
       </c>
@@ -3847,7 +3853,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="198" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>221</v>
       </c>
@@ -3858,7 +3864,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="199" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>221</v>
       </c>
@@ -3869,7 +3875,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="200" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>221</v>
       </c>
@@ -3880,7 +3886,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>221</v>
       </c>
@@ -3891,7 +3897,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>221</v>
       </c>
@@ -3902,7 +3908,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>221</v>
       </c>
@@ -3913,7 +3919,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>221</v>
       </c>
@@ -3924,7 +3930,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>221</v>
       </c>
@@ -3935,7 +3941,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>221</v>
       </c>
@@ -3946,7 +3952,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>221</v>
       </c>
@@ -3957,7 +3963,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>221</v>
       </c>
@@ -3968,7 +3974,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>221</v>
       </c>
@@ -3982,7 +3988,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>221</v>
       </c>
@@ -3993,7 +3999,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>221</v>
       </c>
@@ -4004,7 +4010,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="212" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>221</v>
       </c>
@@ -4015,7 +4021,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>221</v>
       </c>
@@ -4026,7 +4032,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>221</v>
       </c>
@@ -4037,7 +4043,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>221</v>
       </c>
@@ -4048,7 +4054,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>303</v>
       </c>
@@ -4059,7 +4065,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>303</v>
       </c>
@@ -4073,7 +4079,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>303</v>
       </c>
@@ -4084,7 +4090,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>303</v>
       </c>
@@ -4095,7 +4101,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>303</v>
       </c>
@@ -4106,7 +4112,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="221" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>303</v>
       </c>
@@ -4117,7 +4123,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>303</v>
       </c>
@@ -4128,7 +4134,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>303</v>
       </c>
@@ -4139,7 +4145,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>303</v>
       </c>
@@ -4150,7 +4156,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>303</v>
       </c>
@@ -4161,7 +4167,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>303</v>
       </c>
@@ -4172,7 +4178,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>303</v>
       </c>
@@ -4183,7 +4189,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>303</v>
       </c>
@@ -4194,7 +4200,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>303</v>
       </c>
@@ -4205,7 +4211,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>303</v>
       </c>
@@ -4216,7 +4222,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>303</v>
       </c>
@@ -4227,7 +4233,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>303</v>
       </c>
@@ -4238,7 +4244,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>303</v>
       </c>
@@ -4249,7 +4255,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>303</v>
       </c>
@@ -4260,7 +4266,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>303</v>
       </c>
@@ -4271,7 +4277,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>303</v>
       </c>
@@ -4282,10 +4288,10 @@
         <v>329</v>
       </c>
       <c r="E236" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>303</v>
       </c>
@@ -4296,7 +4302,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>303</v>
       </c>
@@ -4307,7 +4313,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="239" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>334</v>
       </c>
@@ -4321,7 +4327,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>334</v>
       </c>
@@ -4332,7 +4338,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>334</v>
       </c>
@@ -4343,7 +4349,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>334</v>
       </c>
@@ -4354,7 +4360,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>334</v>
       </c>
@@ -4365,7 +4371,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>334</v>
       </c>
@@ -4376,7 +4382,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
         <v>334</v>
       </c>
@@ -4387,7 +4393,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>334</v>
       </c>
@@ -4398,7 +4404,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>334</v>
       </c>
@@ -4409,7 +4415,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="248" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>334</v>
       </c>
@@ -4423,7 +4429,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>334</v>
       </c>
@@ -4434,7 +4440,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>334</v>
       </c>
@@ -4445,7 +4451,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>334</v>
       </c>
@@ -4456,7 +4462,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>334</v>
       </c>
@@ -4467,7 +4473,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>334</v>
       </c>
@@ -4478,7 +4484,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>334</v>
       </c>
@@ -4489,7 +4495,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>334</v>
       </c>
@@ -4500,7 +4506,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="256" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>334</v>
       </c>
@@ -4511,7 +4517,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>334</v>
       </c>
@@ -4522,7 +4528,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>334</v>
       </c>
@@ -4533,7 +4539,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>334</v>
       </c>
@@ -4544,7 +4550,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>334</v>
       </c>
@@ -4555,7 +4561,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>362</v>
       </c>
@@ -4566,7 +4572,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>362</v>
       </c>
@@ -4577,7 +4583,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>362</v>
       </c>
@@ -4588,7 +4594,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>362</v>
       </c>
@@ -4599,7 +4605,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>362</v>
       </c>
@@ -4610,7 +4616,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>362</v>
       </c>
@@ -4621,7 +4627,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>365</v>
       </c>
@@ -4632,7 +4638,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>365</v>
       </c>
@@ -4643,7 +4649,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>365</v>
       </c>
@@ -4654,7 +4660,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>365</v>
       </c>
@@ -4665,7 +4671,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
         <v>365</v>
       </c>
@@ -4676,7 +4682,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>365</v>
       </c>
@@ -4688,7 +4694,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E272" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E272" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="weight_estimated"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to release notes and query vignette plot and summary queries to finalize for v2.0.0 release
</commit_message>
<xml_diff>
--- a/vignettes/cvtdb_field_dictionary.xlsx
+++ b/vignettes/cvtdb_field_dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdbLoad/output/release/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdbLoad/vignettes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="11_95785EC48F79A8D366075C52F37BD2727AC59A03" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFC32BB9-A4F8-46A9-AB36-32E56ECD45FE}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="11_95785EC48F79A8D366075C52F37BD2727AC59A03" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0EC0065-6401-4BB6-99E6-9B9818342A6D}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2355" yWindow="1785" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="496">
   <si>
     <t>table_name</t>
   </si>
@@ -868,9 +868,6 @@
     <t>The maximum value for a plot’s x-axis.</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>Only for series with x and y axes.</t>
   </si>
   <si>
@@ -880,9 +877,6 @@
     <t>The minimum value for a plot’s x-axis.</t>
   </si>
   <si>
-    <t>18</t>
-  </si>
-  <si>
     <t>y_max</t>
   </si>
   <si>
@@ -893,9 +887,6 @@
   </si>
   <si>
     <t>The minimum value for a plot’s y-axis.</t>
-  </si>
-  <si>
-    <t>14</t>
   </si>
   <si>
     <t>studies</t>
@@ -3959,11 +3950,11 @@
       <c r="C157" t="s">
         <v>280</v>
       </c>
-      <c r="D157" t="s">
+      <c r="D157">
+        <v>18</v>
+      </c>
+      <c r="E157" t="s">
         <v>281</v>
-      </c>
-      <c r="E157" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -3971,16 +3962,16 @@
         <v>213</v>
       </c>
       <c r="B158" t="s">
+        <v>282</v>
+      </c>
+      <c r="C158" t="s">
         <v>283</v>
       </c>
-      <c r="C158" t="s">
-        <v>284</v>
-      </c>
-      <c r="D158" t="s">
-        <v>285</v>
+      <c r="D158">
+        <v>0</v>
       </c>
       <c r="E158" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -3988,16 +3979,16 @@
         <v>213</v>
       </c>
       <c r="B159" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C159" t="s">
-        <v>287</v>
-      </c>
-      <c r="D159" t="s">
+        <v>285</v>
+      </c>
+      <c r="D159">
+        <v>14</v>
+      </c>
+      <c r="E159" t="s">
         <v>281</v>
-      </c>
-      <c r="E159" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -4005,146 +3996,146 @@
         <v>213</v>
       </c>
       <c r="B160" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C160" t="s">
-        <v>289</v>
-      </c>
-      <c r="D160" t="s">
-        <v>290</v>
+        <v>287</v>
+      </c>
+      <c r="D160">
+        <v>0</v>
       </c>
       <c r="E160" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B161" t="s">
         <v>9</v>
       </c>
       <c r="C161" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D161" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B162" t="s">
         <v>27</v>
       </c>
       <c r="C162" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D162" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B163" t="s">
         <v>33</v>
       </c>
       <c r="C163" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D163" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B164" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C164" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D164" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B165" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C165" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D165" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B166" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C166" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B167" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C167" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B168" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C168" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B169" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C169" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B170" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C170" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B171" t="s">
         <v>224</v>
@@ -4153,49 +4144,49 @@
         <v>225</v>
       </c>
       <c r="D171" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B172" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C172" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D172" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B173" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C173" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D173" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B174" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C174" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D174" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E174" t="s">
         <v>261</v>
@@ -4203,13 +4194,13 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B175" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C175" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D175" t="s">
         <v>143</v>
@@ -4217,7 +4208,7 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B176" t="s">
         <v>18</v>
@@ -4228,7 +4219,7 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B177" t="s">
         <v>91</v>
@@ -4237,71 +4228,71 @@
         <v>92</v>
       </c>
       <c r="D177" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B178" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C178" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D178" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B179" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C179" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D179" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B180" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C180" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B181" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C181" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D181" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B182" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C182" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D182" t="s">
         <v>278</v>
@@ -4309,289 +4300,289 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B183" t="s">
         <v>211</v>
       </c>
       <c r="C183" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D183" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B184" t="s">
+        <v>339</v>
+      </c>
+      <c r="C184" t="s">
+        <v>340</v>
+      </c>
+      <c r="D184" t="s">
+        <v>341</v>
+      </c>
+      <c r="E184" t="s">
         <v>342</v>
-      </c>
-      <c r="C184" t="s">
-        <v>343</v>
-      </c>
-      <c r="D184" t="s">
-        <v>344</v>
-      </c>
-      <c r="E184" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B185" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C185" t="s">
         <v>10</v>
       </c>
       <c r="D185" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="E185" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B186" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C186" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D186" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B187" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C187" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D187" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B188" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C188" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D188" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B189" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C189" t="s">
         <v>10</v>
       </c>
       <c r="D189" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B190" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C190" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D190" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B191" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C191" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D191" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B192" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C192" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D192" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B193" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C193" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D193" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B194" t="s">
+        <v>368</v>
+      </c>
+      <c r="C194" t="s">
+        <v>369</v>
+      </c>
+      <c r="D194" t="s">
+        <v>370</v>
+      </c>
+      <c r="E194" t="s">
         <v>371</v>
-      </c>
-      <c r="C194" t="s">
-        <v>372</v>
-      </c>
-      <c r="D194" t="s">
-        <v>373</v>
-      </c>
-      <c r="E194" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B195" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C195" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B196" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C196" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B197" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C197" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B198" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C198" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B199" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C199" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B200" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C200" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B201" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C201" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B202" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C202" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D202" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B203" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C203" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D203" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B204" t="s">
         <v>20</v>
@@ -4602,21 +4593,21 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B205" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C205" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D205" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B206" t="s">
         <v>99</v>
@@ -4625,12 +4616,12 @@
         <v>100</v>
       </c>
       <c r="D206" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B207" t="s">
         <v>101</v>
@@ -4639,12 +4630,12 @@
         <v>102</v>
       </c>
       <c r="D207" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B208" t="s">
         <v>103</v>
@@ -4658,7 +4649,7 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B209" t="s">
         <v>22</v>
@@ -4669,13 +4660,13 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B210" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C210" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D210" t="s">
         <v>143</v>
@@ -4683,77 +4674,77 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B211" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C211" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="D211" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B212" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C212" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D212" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B213" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C213" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D213" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B214" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C214" t="s">
+        <v>405</v>
+      </c>
+      <c r="D214" t="s">
         <v>408</v>
-      </c>
-      <c r="D214" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B215" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C215" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D215" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B216" t="s">
         <v>108</v>
@@ -4764,49 +4755,49 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
+        <v>411</v>
+      </c>
+      <c r="B217" t="s">
+        <v>412</v>
+      </c>
+      <c r="C217" t="s">
+        <v>413</v>
+      </c>
+      <c r="D217" t="s">
         <v>414</v>
-      </c>
-      <c r="B217" t="s">
-        <v>415</v>
-      </c>
-      <c r="C217" t="s">
-        <v>416</v>
-      </c>
-      <c r="D217" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B218" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C218" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D218" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B219" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C219" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D219" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B220" t="s">
         <v>18</v>
@@ -4817,7 +4808,7 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B221" t="s">
         <v>91</v>
@@ -4826,68 +4817,68 @@
         <v>92</v>
       </c>
       <c r="D221" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B222" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C222" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="D222" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B223" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C223" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D223" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B224" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C224" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D224" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B225" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C225" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="D225" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B226" t="s">
         <v>20</v>
@@ -4898,24 +4889,24 @@
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B227" t="s">
         <v>4</v>
       </c>
       <c r="C227" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D227" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="E227" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B228" t="s">
         <v>99</v>
@@ -4924,12 +4915,12 @@
         <v>100</v>
       </c>
       <c r="D228" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B229" t="s">
         <v>101</v>
@@ -4938,12 +4929,12 @@
         <v>102</v>
       </c>
       <c r="D229" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B230" t="s">
         <v>103</v>
@@ -4957,7 +4948,7 @@
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B231" t="s">
         <v>22</v>
@@ -4968,49 +4959,49 @@
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B232" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C232" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="D232" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B233" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C233" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D233" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B234" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C234" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D234" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B235" t="s">
         <v>108</v>
@@ -5021,55 +5012,55 @@
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B236" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C236" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="D236" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B237" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C237" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D237" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B238" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C238" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="D238" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B239" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C239" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="D239" t="s">
         <v>143</v>
@@ -5077,32 +5068,32 @@
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
+        <v>457</v>
+      </c>
+      <c r="B240" t="s">
         <v>460</v>
       </c>
-      <c r="B240" t="s">
-        <v>463</v>
-      </c>
       <c r="C240" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B241" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C241" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D241" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B242" t="s">
         <v>18</v>
@@ -5113,18 +5104,18 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B243" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="C243" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B244" t="s">
         <v>93</v>
@@ -5135,18 +5126,18 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B245" t="s">
         <v>249</v>
       </c>
       <c r="C245" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B246" t="s">
         <v>20</v>
@@ -5157,24 +5148,24 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B247" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C247" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B248" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="C248" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="D248" t="s">
         <v>143</v>
@@ -5182,63 +5173,63 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B249" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="C249" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="D249" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B250" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C250" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="D250" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B251" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="C251" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="D251" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B252" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="C252" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="D252" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B253" t="s">
         <v>99</v>
@@ -5249,7 +5240,7 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B254" t="s">
         <v>101</v>
@@ -5260,7 +5251,7 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B255" t="s">
         <v>103</v>
@@ -5271,18 +5262,18 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B256" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="C256" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B257" t="s">
         <v>22</v>
@@ -5293,29 +5284,29 @@
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B258" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="C258" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B259" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="C259" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B260" t="s">
         <v>108</v>
@@ -5326,7 +5317,7 @@
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B261" t="s">
         <v>18</v>
@@ -5335,12 +5326,12 @@
         <v>19</v>
       </c>
       <c r="E261" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B262" t="s">
         <v>93</v>
@@ -5349,26 +5340,26 @@
         <v>94</v>
       </c>
       <c r="E262" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
+        <v>490</v>
+      </c>
+      <c r="B263" t="s">
+        <v>492</v>
+      </c>
+      <c r="C263" t="s">
         <v>493</v>
       </c>
-      <c r="B263" t="s">
-        <v>495</v>
-      </c>
-      <c r="C263" t="s">
-        <v>496</v>
-      </c>
       <c r="E263" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B264" t="s">
         <v>20</v>
@@ -5377,12 +5368,12 @@
         <v>21</v>
       </c>
       <c r="E264" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B265" t="s">
         <v>22</v>
@@ -5391,12 +5382,12 @@
         <v>23</v>
       </c>
       <c r="E265" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B266" t="s">
         <v>108</v>
@@ -5405,12 +5396,12 @@
         <v>109</v>
       </c>
       <c r="E266" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B267" t="s">
         <v>18</v>
@@ -5419,40 +5410,40 @@
         <v>19</v>
       </c>
       <c r="E267" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B268" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C268" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="E268" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B269" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C269" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="E269" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B270" t="s">
         <v>20</v>
@@ -5461,12 +5452,12 @@
         <v>21</v>
       </c>
       <c r="E270" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B271" t="s">
         <v>22</v>
@@ -5475,12 +5466,12 @@
         <v>23</v>
       </c>
       <c r="E271" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B272" t="s">
         <v>108</v>
@@ -5489,7 +5480,7 @@
         <v>109</v>
       </c>
       <c r="E272" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
   </sheetData>

</xml_diff>